<commit_message>
acertos no codigo da tabela hash
</commit_message>
<xml_diff>
--- a/Comparativo dos códigos.xlsx
+++ b/Comparativo dos códigos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\IdeaProjects\TrabalhoTPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BEE51E7-2471-43C1-B3EF-652DC46A013B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22AA887-6E22-4C51-8D34-32166165BA7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="2460" windowWidth="28800" windowHeight="12750" xr2:uid="{E0E95DBE-E94F-49ED-B3E3-6D0CDFFBB7B0}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15450" windowHeight="12750" xr2:uid="{E0E95DBE-E94F-49ED-B3E3-6D0CDFFBB7B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha2" sheetId="2" r:id="rId1"/>
@@ -79,7 +79,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -88,7 +88,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.499984740745262"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -121,10 +127,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -280,19 +287,19 @@
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2890</c:v>
+                  <c:v>2813</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9719</c:v>
+                  <c:v>9503</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>178672</c:v>
+                  <c:v>160135</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>714335</c:v>
+                  <c:v>716654</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -361,19 +368,19 @@
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11957</c:v>
+                  <c:v>11999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27489</c:v>
+                  <c:v>29339</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>161796</c:v>
+                  <c:v>174399</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>179123</c:v>
+                  <c:v>341112</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1602,82 +1609,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58446C79-CA82-46DB-867F-045619F60738}">
   <dimension ref="B1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA9" sqref="AA9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>6</v>
       </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>16</v>
+      <c r="C3" s="2">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>1000000</v>
       </c>
-      <c r="C4" s="1">
-        <v>2890</v>
-      </c>
-      <c r="D4" s="1">
-        <v>11957</v>
+      <c r="C4" s="2">
+        <v>2813</v>
+      </c>
+      <c r="D4" s="2">
+        <v>11999</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>2111898</v>
       </c>
-      <c r="C5" s="1">
-        <v>9719</v>
-      </c>
-      <c r="D5" s="1">
-        <v>27489</v>
+      <c r="C5" s="2">
+        <v>9503</v>
+      </c>
+      <c r="D5" s="2">
+        <v>29339</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>9999741</v>
       </c>
-      <c r="C6" s="1">
-        <v>178672</v>
-      </c>
-      <c r="D6" s="1">
-        <v>161796</v>
+      <c r="C6" s="2">
+        <v>160135</v>
+      </c>
+      <c r="D6" s="2">
+        <v>174399</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>19999783</v>
       </c>
-      <c r="C7" s="1">
-        <v>714335</v>
-      </c>
-      <c r="D7" s="1">
-        <v>179123</v>
+      <c r="C7" s="2">
+        <v>716654</v>
+      </c>
+      <c r="D7" s="2">
+        <v>341112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>